<commit_message>
Dashboard Filter Bulan And PPN Settings
* fitur ++

* fitur ++++

* dashboard fix
</commit_message>
<xml_diff>
--- a/public/assets/report/transaksi.xlsx
+++ b/public/assets/report/transaksi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fahmi\Dev\laundry\public\assets\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C05AE6B-1748-4B4F-8186-F310CC42477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F14EB4-09DE-4CB8-8B4F-9BDEA9353A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>timestamp</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Biaya Tambahan</t>
+  </si>
+  <si>
+    <t>PPN</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -491,24 +494,24 @@
     <col min="7" max="7" width="10.140625" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" customWidth="1"/>
     <col min="18" max="18" width="5.42578125" customWidth="1"/>
     <col min="19" max="19" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -516,17 +519,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -567,6 +570,9 @@
         <v>18</v>
       </c>
       <c r="N7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>